<commit_message>
Modifed excel in dealerconfiguration
</commit_message>
<xml_diff>
--- a/configs/DealerConfiguration/dinesharora80.xlsx
+++ b/configs/DealerConfiguration/dinesharora80.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="35">
   <si>
     <t>Dealer Number</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 </t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -173,6 +176,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,7 +492,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A23" sqref="A23:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,8 +749,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>8</v>
+      <c r="A11" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>

</xml_diff>